<commit_message>
completed implementation of joinCsv
</commit_message>
<xml_diff>
--- a/xlsxToCsv/data/DistTableDisplay6b - 0.xlsx
+++ b/xlsxToCsv/data/DistTableDisplay6b - 0.xlsx
@@ -139,17 +139,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -227,6 +216,19 @@
       <top style="thin">
         <color rgb="FFFFFFFF"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -275,7 +277,7 @@
   <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf applyFont="1" applyFill="1" applyBorder="1" numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="2" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
@@ -295,13 +297,10 @@
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="1" fillId="0" borderId="2">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="4" fillId="2" borderId="3">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="1" fillId="0" borderId="3">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="5" fillId="2" borderId="3">
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="5" fillId="2" borderId="2">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="5" fillId="3" borderId="3">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="5" fillId="3" borderId="4">
@@ -447,29 +446,31 @@
     <sheetView workbookViewId="0" showGridLines="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" customWidth="1" width="13.6640625"/>
-    <col min="2" max="2" customWidth="1" width="50.2421875"/>
-    <col min="3" max="3" customWidth="1" width="39.1015625"/>
-    <col min="4" max="4" customWidth="1" width="38.51171875"/>
-    <col min="5" max="5" customWidth="1" width="41.6640625"/>
-    <col min="6" max="6" customWidth="1" width="0.29296875"/>
-    <col min="7" max="7" customWidth="1" width="3.703125"/>
+    <col min="1" max="1" customWidth="1" width="13.61328125"/>
+    <col min="2" max="2" customWidth="1" width="47.18359375"/>
+    <col min="3" max="3" customWidth="1" width="31.453125"/>
+    <col min="4" max="4" customWidth="1" width="30.6328125"/>
+    <col min="5" max="5" customWidth="1" width="30.453125"/>
+    <col min="6" max="6" customWidth="1" width="33.18359375"/>
+    <col min="7" max="7" customWidth="1" width="0.29296875"/>
+    <col min="8" max="8" customWidth="1" width="0.390625"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.2" customHeight="1"/>
-    <row r="2" ht="4" customHeight="1"/>
-    <row r="3" ht="25.8" customHeight="1">
+    <row r="2" ht="1" customHeight="1"/>
+    <row r="3" ht="21.75" customHeight="1">
       <c s="1" t="inlineStr" r="A3">
         <is>
-          <t xml:space="preserve">AGRICULTURAL CENSUS , 1995-96</t>
+          <t xml:space="preserve">AGRICULTURAL CENSUS , 2005-06</t>
         </is>
       </c>
       <c s="2" t="str" r="B3"/>
       <c s="2" t="str" r="C3"/>
       <c s="2" t="str" r="D3"/>
       <c s="2" t="str" r="E3"/>
-    </row>
-    <row r="4" ht="17.6" customHeight="1">
+      <c s="2" t="str" r="F3"/>
+    </row>
+    <row r="4" ht="17.25" customHeight="1">
       <c s="3" t="inlineStr" r="A4">
         <is>
           <r>
@@ -502,8 +503,9 @@
       <c s="2" t="str" r="C4"/>
       <c s="2" t="str" r="D4"/>
       <c s="2" t="str" r="E4"/>
-    </row>
-    <row r="5" ht="17.55" customHeight="0">
+      <c s="2" t="str" r="F4"/>
+    </row>
+    <row r="5" ht="17.25" customHeight="1">
       <c s="4" t="inlineStr" r="A5">
         <is>
           <r>
@@ -590,447 +592,518 @@
           </r>
         </is>
       </c>
-    </row>
-    <row r="6" ht="17.6" customHeight="0">
+      <c s="2" t="str" r="F5"/>
+    </row>
+    <row r="6" ht="17.3" customHeight="0">
       <c s="5" t="inlineStr" r="A6">
         <is>
           <t xml:space="preserve">NUMBER IN  ABSOLUTE UNITS</t>
         </is>
       </c>
       <c s="6" t="str" r="B6"/>
-      <c s="7" t="inlineStr" r="C6">
+      <c s="5" t="inlineStr" r="C6">
         <is>
           <t xml:space="preserve">AREA IN  HECTARES</t>
         </is>
       </c>
-      <c s="8" t="str" r="D6"/>
-      <c s="9" t="inlineStr" r="E6">
+      <c s="6" t="str" r="D6"/>
+      <c s="7" t="inlineStr" r="E6">
         <is>
           <t xml:space="preserve"/>
         </is>
       </c>
-    </row>
-    <row r="7" ht="32.4" customHeight="0">
-      <c s="10" t="inlineStr" r="A7">
-        <is>
-          <t xml:space="preserve">Sl.No.</t>
-        </is>
-      </c>
-      <c s="11" t="inlineStr" r="B7">
+      <c s="7" t="inlineStr" r="F6">
+        <is>
+          <t xml:space="preserve"/>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="0">
+      <c s="8" t="inlineStr" r="A7">
+        <is>
+          <t xml:space="preserve">Sl No</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="B7">
         <is>
           <t xml:space="preserve">Size Class(HA)</t>
         </is>
       </c>
-      <c s="11" t="inlineStr" r="C7">
+      <c s="9" t="inlineStr" r="C7">
+        <is>
+          <t xml:space="preserve">No. of Holdings</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="D7">
         <is>
           <t xml:space="preserve">Irrigated Area</t>
         </is>
       </c>
-      <c s="11" t="inlineStr" r="D7">
-        <is>
-          <t xml:space="preserve">Unirrigated Area</t>
-        </is>
-      </c>
-      <c s="12" t="inlineStr" r="E7">
+      <c s="9" t="inlineStr" r="E7">
+        <is>
+          <t xml:space="preserve">Unirrigated Area </t>
+        </is>
+      </c>
+      <c s="10" t="inlineStr" r="F7">
         <is>
           <t xml:space="preserve">Total Area</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="22.85" customHeight="0">
-      <c s="13" t="inlineStr" r="A8">
+    <row r="8" ht="21.75" customHeight="0">
+      <c s="11" t="inlineStr" r="A8">
         <is>
           <t xml:space="preserve">(1)</t>
         </is>
       </c>
-      <c s="14" t="inlineStr" r="B8">
+      <c s="12" t="inlineStr" r="B8">
         <is>
           <t xml:space="preserve">(2)</t>
         </is>
       </c>
-      <c s="14" t="inlineStr" r="C8">
+      <c s="13" t="inlineStr" r="C8">
         <is>
           <t xml:space="preserve">(3)</t>
         </is>
       </c>
-      <c s="14" t="inlineStr" r="D8">
+      <c s="12" t="inlineStr" r="D8">
         <is>
           <t xml:space="preserve">(4)</t>
         </is>
       </c>
-      <c s="15" t="inlineStr" r="E8">
+      <c s="12" t="inlineStr" r="E8">
         <is>
           <t xml:space="preserve">(5)</t>
         </is>
       </c>
-    </row>
-    <row r="9" ht="19.65" customHeight="0">
-      <c s="16" t="inlineStr" r="A9">
+      <c s="14" t="inlineStr" r="F8">
+        <is>
+          <t xml:space="preserve">(6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="18.75" customHeight="0">
+      <c s="15" t="inlineStr" r="A9">
         <is>
           <t xml:space="preserve"> 1</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B9">
+      <c s="16" t="inlineStr" r="B9">
         <is>
           <t xml:space="preserve">Below 0.5</t>
         </is>
       </c>
-      <c s="18" r="C9">
-        <v>0</v>
-      </c>
-      <c s="18" r="D9">
-        <v>214</v>
-      </c>
-      <c s="18" r="E9">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" ht="19.7" customHeight="0">
-      <c s="16" t="inlineStr" r="A10">
+      <c s="17" r="C9">
+        <v>2870</v>
+      </c>
+      <c s="17" r="D9">
+        <v>0</v>
+      </c>
+      <c s="17" r="E9">
+        <v>178</v>
+      </c>
+      <c s="17" r="F9">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" ht="18.75" customHeight="0">
+      <c s="15" t="inlineStr" r="A10">
         <is>
           <t xml:space="preserve">2</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B10">
+      <c s="16" t="inlineStr" r="B10">
         <is>
           <t xml:space="preserve">0.5 - 1.0</t>
         </is>
       </c>
-      <c s="18" r="C10">
-        <v>0</v>
-      </c>
-      <c s="18" r="D10">
-        <v>515</v>
-      </c>
-      <c s="18" r="E10">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="11" ht="19.7" customHeight="0">
-      <c s="19" t="inlineStr" r="A11">
+      <c s="17" r="C10">
+        <v>2761</v>
+      </c>
+      <c s="17" r="D10">
+        <v>0</v>
+      </c>
+      <c s="17" r="E10">
+        <v>631</v>
+      </c>
+      <c s="17" r="F10">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="11" ht="18.75" customHeight="0">
+      <c s="18" t="inlineStr" r="A11">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c s="20" t="inlineStr" r="B11">
+      <c s="19" t="inlineStr" r="B11">
         <is>
           <t xml:space="preserve">MARGINAL</t>
         </is>
       </c>
-      <c s="21" r="C11">
-        <v>0</v>
-      </c>
-      <c s="21" r="D11">
-        <v>729</v>
-      </c>
-      <c s="21" r="E11">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="12" ht="19.7" customHeight="0">
-      <c s="16" t="inlineStr" r="A12">
+      <c s="20" r="C11">
+        <v>5631</v>
+      </c>
+      <c s="20" r="D11">
+        <v>0</v>
+      </c>
+      <c s="20" r="E11">
+        <v>809</v>
+      </c>
+      <c s="20" r="F11">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="12" ht="18.8" customHeight="0">
+      <c s="15" t="inlineStr" r="A12">
         <is>
           <t xml:space="preserve">3</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B12">
+      <c s="16" t="inlineStr" r="B12">
         <is>
           <t xml:space="preserve">1.0 - 2.0</t>
         </is>
       </c>
-      <c s="18" r="C12">
-        <v>0</v>
-      </c>
-      <c s="18" r="D12">
-        <v>2582</v>
-      </c>
-      <c s="18" r="E12">
-        <v>2582</v>
-      </c>
-    </row>
-    <row r="13" ht="19.65" customHeight="0">
-      <c s="19" t="inlineStr" r="A13">
+      <c s="17" r="C12">
+        <v>3564</v>
+      </c>
+      <c s="17" r="D12">
+        <v>0</v>
+      </c>
+      <c s="17" r="E12">
+        <v>1496</v>
+      </c>
+      <c s="17" r="F12">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="13" ht="18.75" customHeight="0">
+      <c s="18" t="inlineStr" r="A13">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c s="20" t="inlineStr" r="B13">
+      <c s="19" t="inlineStr" r="B13">
         <is>
           <t xml:space="preserve">SMALL</t>
         </is>
       </c>
-      <c s="21" r="C13">
-        <v>0</v>
-      </c>
-      <c s="21" r="D13">
-        <v>2582</v>
-      </c>
-      <c s="21" r="E13">
-        <v>2582</v>
-      </c>
-    </row>
-    <row r="14" ht="19.7" customHeight="0">
-      <c s="16" t="inlineStr" r="A14">
+      <c s="20" r="C13">
+        <v>3564</v>
+      </c>
+      <c s="20" r="D13">
+        <v>0</v>
+      </c>
+      <c s="20" r="E13">
+        <v>1496</v>
+      </c>
+      <c s="20" r="F13">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="14" ht="18.75" customHeight="0">
+      <c s="15" t="inlineStr" r="A14">
         <is>
           <t xml:space="preserve">4</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B14">
+      <c s="16" t="inlineStr" r="B14">
         <is>
           <t xml:space="preserve">2.0 - 3.0</t>
         </is>
       </c>
-      <c s="18" r="C14">
-        <v>0</v>
-      </c>
-      <c s="18" r="D14">
-        <v>4278</v>
-      </c>
-      <c s="18" r="E14">
-        <v>4278</v>
-      </c>
-    </row>
-    <row r="15" ht="19.7" customHeight="0">
-      <c s="16" t="inlineStr" r="A15">
+      <c s="17" r="C14">
+        <v>3454</v>
+      </c>
+      <c s="17" r="D14">
+        <v>0</v>
+      </c>
+      <c s="17" r="E14">
+        <v>1753</v>
+      </c>
+      <c s="17" r="F14">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="15" ht="18.75" customHeight="0">
+      <c s="15" t="inlineStr" r="A15">
         <is>
           <t xml:space="preserve">5</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B15">
+      <c s="16" t="inlineStr" r="B15">
         <is>
           <t xml:space="preserve">3.0 - 4.0</t>
         </is>
       </c>
-      <c s="18" r="C15">
-        <v>0</v>
-      </c>
-      <c s="18" r="D15">
-        <v>1925</v>
-      </c>
-      <c s="18" r="E15">
-        <v>1925</v>
-      </c>
-    </row>
-    <row r="16" ht="19.7" customHeight="0">
-      <c s="19" t="inlineStr" r="A16">
+      <c s="17" r="C15">
+        <v>795</v>
+      </c>
+      <c s="17" r="D15">
+        <v>0</v>
+      </c>
+      <c s="17" r="E15">
+        <v>459</v>
+      </c>
+      <c s="17" r="F15">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="16" ht="18.75" customHeight="0">
+      <c s="18" t="inlineStr" r="A16">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c s="20" t="inlineStr" r="B16">
+      <c s="19" t="inlineStr" r="B16">
         <is>
           <t xml:space="preserve">SEMIMEDIUM</t>
         </is>
       </c>
-      <c s="21" r="C16">
-        <v>0</v>
-      </c>
-      <c s="21" r="D16">
-        <v>6203</v>
-      </c>
-      <c s="21" r="E16">
-        <v>6203</v>
-      </c>
-    </row>
-    <row r="17" ht="19.65" customHeight="0">
-      <c s="16" t="inlineStr" r="A17">
+      <c s="20" r="C16">
+        <v>4249</v>
+      </c>
+      <c s="20" r="D16">
+        <v>0</v>
+      </c>
+      <c s="20" r="E16">
+        <v>2212</v>
+      </c>
+      <c s="20" r="F16">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="17" ht="18.75" customHeight="0">
+      <c s="15" t="inlineStr" r="A17">
         <is>
           <t xml:space="preserve">6</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B17">
+      <c s="16" t="inlineStr" r="B17">
         <is>
           <t xml:space="preserve">4.0 - 5.0</t>
         </is>
       </c>
-      <c s="18" r="C17">
-        <v>0</v>
-      </c>
-      <c s="18" r="D17">
-        <v>4562</v>
-      </c>
-      <c s="18" r="E17">
-        <v>4562</v>
-      </c>
-    </row>
-    <row r="18" ht="19.7" customHeight="0">
-      <c s="16" t="inlineStr" r="A18">
+      <c s="17" r="C17">
+        <v>453</v>
+      </c>
+      <c s="17" r="D17">
+        <v>0</v>
+      </c>
+      <c s="17" r="E17">
+        <v>306</v>
+      </c>
+      <c s="17" r="F17">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" ht="18.8" customHeight="0">
+      <c s="15" t="inlineStr" r="A18">
         <is>
           <t xml:space="preserve">7</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B18">
+      <c s="16" t="inlineStr" r="B18">
         <is>
           <t xml:space="preserve">5.0 - 7.5</t>
         </is>
       </c>
-      <c s="18" r="C18">
-        <v>0</v>
-      </c>
-      <c s="18" r="D18">
-        <v>226</v>
-      </c>
-      <c s="18" r="E18">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="19" ht="19.7" customHeight="0">
-      <c s="16" t="inlineStr" r="A19">
+      <c s="17" r="C18">
+        <v>166</v>
+      </c>
+      <c s="17" r="D18">
+        <v>0</v>
+      </c>
+      <c s="17" r="E18">
+        <v>145</v>
+      </c>
+      <c s="17" r="F18">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75" customHeight="0">
+      <c s="15" t="inlineStr" r="A19">
         <is>
           <t xml:space="preserve">8</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B19">
+      <c s="16" t="inlineStr" r="B19">
         <is>
           <t xml:space="preserve">7.5 - 10.0</t>
         </is>
       </c>
-      <c s="18" r="C19">
-        <v>0</v>
-      </c>
-      <c s="18" r="D19">
-        <v>82</v>
-      </c>
-      <c s="18" r="E19">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" ht="19.7" customHeight="0">
-      <c s="19" t="inlineStr" r="A20">
+      <c s="17" r="C19">
+        <v>81</v>
+      </c>
+      <c s="17" r="D19">
+        <v>0</v>
+      </c>
+      <c s="17" r="E19">
+        <v>85</v>
+      </c>
+      <c s="17" r="F19">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" ht="18.75" customHeight="0">
+      <c s="18" t="inlineStr" r="A20">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c s="20" t="inlineStr" r="B20">
+      <c s="19" t="inlineStr" r="B20">
         <is>
           <t xml:space="preserve">MEDIUM</t>
         </is>
       </c>
-      <c s="21" r="C20">
-        <v>0</v>
-      </c>
-      <c s="21" r="D20">
-        <v>4870</v>
-      </c>
-      <c s="21" r="E20">
-        <v>4870</v>
-      </c>
-    </row>
-    <row r="21" ht="19.65" customHeight="0">
-      <c s="16" t="inlineStr" r="A21">
+      <c s="20" r="C20">
+        <v>700</v>
+      </c>
+      <c s="20" r="D20">
+        <v>0</v>
+      </c>
+      <c s="20" r="E20">
+        <v>536</v>
+      </c>
+      <c s="20" r="F20">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="21" ht="18.75" customHeight="0">
+      <c s="15" t="inlineStr" r="A21">
         <is>
           <t xml:space="preserve">9</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B21">
+      <c s="16" t="inlineStr" r="B21">
         <is>
           <t xml:space="preserve">10.0 - 20.0</t>
         </is>
       </c>
-      <c s="18" r="C21">
-        <v>0</v>
-      </c>
-      <c s="18" r="D21">
-        <v>243</v>
-      </c>
-      <c s="18" r="E21">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="22" ht="19.7" customHeight="0">
-      <c s="16" t="inlineStr" r="A22">
+      <c s="17" r="C21">
+        <v>20</v>
+      </c>
+      <c s="17" r="D21">
+        <v>0</v>
+      </c>
+      <c s="17" r="E21">
+        <v>63</v>
+      </c>
+      <c s="17" r="F21">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" ht="18.75" customHeight="0">
+      <c s="15" t="inlineStr" r="A22">
         <is>
           <t xml:space="preserve">10</t>
         </is>
       </c>
-      <c s="17" t="inlineStr" r="B22">
+      <c s="16" t="inlineStr" r="B22">
         <is>
           <t xml:space="preserve">20.0 &amp; ABOVE</t>
         </is>
       </c>
-      <c s="18" r="C22">
-        <v>0</v>
-      </c>
-      <c s="18" r="D22">
-        <v>1203</v>
-      </c>
-      <c s="18" r="E22">
-        <v>1203</v>
-      </c>
-    </row>
-    <row r="23" ht="19.7" customHeight="0">
-      <c s="19" t="inlineStr" r="A23">
+      <c s="17" r="C22">
+        <v>28</v>
+      </c>
+      <c s="17" r="D22">
+        <v>0</v>
+      </c>
+      <c s="17" r="E22">
+        <v>892</v>
+      </c>
+      <c s="17" r="F22">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="23" ht="18.75" customHeight="0">
+      <c s="18" t="inlineStr" r="A23">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c s="20" t="inlineStr" r="B23">
+      <c s="19" t="inlineStr" r="B23">
         <is>
           <t xml:space="preserve">LARGE</t>
         </is>
       </c>
-      <c s="21" r="C23">
-        <v>0</v>
-      </c>
-      <c s="21" r="D23">
-        <v>1446</v>
-      </c>
-      <c s="21" r="E23">
-        <v>1446</v>
-      </c>
-    </row>
-    <row r="24" ht="19.7" customHeight="0">
-      <c s="22" t="inlineStr" r="A24">
+      <c s="20" r="C23">
+        <v>48</v>
+      </c>
+      <c s="20" r="D23">
+        <v>0</v>
+      </c>
+      <c s="20" r="E23">
+        <v>955</v>
+      </c>
+      <c s="20" r="F23">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="24" ht="18.75" customHeight="0">
+      <c s="21" t="inlineStr" r="A24">
         <is>
           <t xml:space="preserve">11</t>
         </is>
       </c>
-      <c s="23" t="inlineStr" r="B24">
+      <c s="22" t="inlineStr" r="B24">
         <is>
           <t xml:space="preserve">ALL CLASSES</t>
         </is>
       </c>
-      <c s="24" r="C24">
-        <v>0</v>
-      </c>
-      <c s="24" r="D24">
-        <v>15830</v>
-      </c>
-      <c s="24" r="E24">
-        <v>15830</v>
-      </c>
-    </row>
-    <row r="25" ht="17.55" customHeight="0">
-      <c s="25" t="inlineStr" r="A25">
+      <c s="23" r="C24">
+        <v>14192</v>
+      </c>
+      <c s="23" r="D24">
+        <v>0</v>
+      </c>
+      <c s="23" r="E24">
+        <v>6009</v>
+      </c>
+      <c s="23" r="F24">
+        <v>6009</v>
+      </c>
+    </row>
+    <row r="25" ht="17.25" customHeight="0">
+      <c s="24" t="inlineStr" r="A25">
         <is>
           <t xml:space="preserve">Note: Total May not Tally Due to Rounding off</t>
         </is>
       </c>
-      <c s="26" t="str" r="B25"/>
-      <c s="27" t="inlineStr" r="C25">
+      <c s="25" t="str" r="B25"/>
+      <c s="26" t="inlineStr" r="C25">
         <is>
           <t xml:space="preserve"/>
         </is>
       </c>
-      <c s="27" t="inlineStr" r="D25">
+      <c s="26" t="inlineStr" r="D25">
         <is>
           <t xml:space="preserve"/>
         </is>
       </c>
-      <c s="28" t="inlineStr" r="E25">
+      <c s="26" t="inlineStr" r="E25">
+        <is>
+          <t xml:space="preserve"/>
+        </is>
+      </c>
+      <c s="27" t="inlineStr" r="F25">
         <is>
           <t xml:space="preserve">Neg:-Negligible</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="1.7" customHeight="1"/>
-    <row r="27" ht="3.7" customHeight="1"/>
+    <row r="26" ht="0.05" customHeight="1"/>
+    <row r="27" ht="4.7" customHeight="1"/>
+    <row r="28" ht="3.7" customHeight="1"/>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A25:B25"/>

</xml_diff>